<commit_message>
jc branch 2 update
</commit_message>
<xml_diff>
--- a/data/sckjc_spring2025.xlsx
+++ b/data/sckjc_spring2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sblanche/Desktop/GitHub/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB08EA8A-1EF4-7641-A1B7-7C0FCC4282AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E376B743-FB3D-D24B-BF53-35DCA2144DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{7D187901-E6A1-4676-A790-E8B1B18E73F2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17260" xr2:uid="{7D187901-E6A1-4676-A790-E8B1B18E73F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,18 +83,12 @@
     <t>Sparsentan improves glomerular hemodynamics, cell functions, and tissue repair in a mouse model of FSGS</t>
   </si>
   <si>
-    <t>JCL Insight 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://pubmed.ncbi.nlm.nih.gov/35522041/ </t>
   </si>
   <si>
     <t xml:space="preserve">https://pubmed.ncbi.nlm.nih.gov/38996810/ </t>
   </si>
   <si>
-    <t xml:space="preserve">https://insight.jci.org/articles/view/177775 </t>
-  </si>
-  <si>
     <t xml:space="preserve">April 1st </t>
   </si>
   <si>
@@ -102,6 +96,12 @@
   </si>
   <si>
     <t>June 3rd</t>
+  </si>
+  <si>
+    <t>JCI Insight 2024</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/39226116/</t>
   </si>
 </sst>
 </file>
@@ -522,7 +522,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -560,7 +560,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>7</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
@@ -586,7 +586,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>8</v>
@@ -594,16 +594,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>9</v>
@@ -624,8 +624,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{FBBB6B41-62E5-7E48-9545-71226C51B9CA}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{6FFE0D09-2418-9F4F-B05A-A7FEE033AAE8}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{F22D9594-387E-AE4F-8284-A8E0D669BDD5}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{F22D9594-387E-AE4F-8284-A8E0D669BDD5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>